<commit_message>
Add labels, an entry, and a button widget
</commit_message>
<xml_diff>
--- a/assets/data/drugs.xlsx
+++ b/assets/data/drugs.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/368813f78804d80c/Desktop/Project AtBS/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="10_ncr:8000_{1F15FA52-845D-4433-9532-B7D85397CB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C7B3AB8-5855-475E-AD2F-27C952524864}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="10_ncr:8000_{1F15FA52-845D-4433-9532-B7D85397CB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BD91D4B-9ADC-4EEA-9BA6-D8E397FDDE9D}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="6960" windowWidth="20985" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8685" yWindow="1635" windowWidth="20985" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="specialty" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">specialty!$A$1:$C$4132</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">specialty!$A$1:$B$4132</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8265" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8264" uniqueCount="774">
   <si>
     <t>Item</t>
   </si>
@@ -2345,9 +2345,6 @@
   </si>
   <si>
     <t>NDC</t>
-  </si>
-  <si>
-    <t>Drop Ship</t>
   </si>
 </sst>
 </file>
@@ -2415,6 +2412,10 @@
 </file>
 
 <file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -2715,31 +2716,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4132"/>
+  <dimension ref="A1:B4132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="84.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>773</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2747,7 +2744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2755,7 +2752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2763,7 +2760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2771,7 +2768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2779,7 +2776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2787,7 +2784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2795,7 +2792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2803,7 +2800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2811,7 +2808,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2819,7 +2816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2827,7 +2824,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2835,7 +2832,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2843,7 +2840,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -2851,7 +2848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -35788,7 +35785,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C4132" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:B4132" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>